<commit_message>
Updated with protocol links
</commit_message>
<xml_diff>
--- a/tascu.xlsx
+++ b/tascu.xlsx
@@ -5090,31 +5090,11 @@
           <t>***** SEVA/METABRICK, Moclo, Gibson pathway engineering @Wageningen</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="H98" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="K98" t="inlineStr">
         <is>
           <t>NULL</t>
@@ -5125,38 +5105,23 @@
       </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>2019-10-11 11:23:41</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B99">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>****** #TODO add the list of tasks needed #ToBeReviewed</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>NULL</t>
+          <t>***** Vector, promoter selection, plasmids, locus of integration, restriction sites, etc (cloning strategy) #SopNeeded</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -5164,11 +5129,6 @@
           <t>NULL</t>
         </is>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="K99" t="inlineStr">
         <is>
           <t>NULL</t>
@@ -5179,38 +5139,33 @@
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>2019-10-11 11:23:41</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100">
+        <v>400</v>
+      </c>
+      <c r="B100">
         <v>67</v>
       </c>
-      <c r="B100">
-        <v>64</v>
-      </c>
       <c r="C100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>***** Vector, promoter selection, plasmids, locus of integration, restriction sites, etc (cloning strategy) #SopNeeded</t>
+          <t>****** Select primers for vector assembly</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>NULL</t>
+          <t>Primers required for construction of the vector</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>https://hub.ibisba.eu/sops/58</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -5218,22 +5173,17 @@
           <t>NULL</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="K100" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
       </c>
       <c r="L100" s="2">
-        <v>43418.5925</v>
+        <v>43749.47356481482</v>
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>2019-10-11 11:26:03</t>
         </is>
       </c>
     </row>
@@ -5252,31 +5202,11 @@
           <t>***** Combinatorial assembly strategy #SopNeeded</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="H101" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="K101" t="inlineStr">
         <is>
           <t>NULL</t>
@@ -5287,7 +5217,7 @@
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>2019-10-11 11:23:41</t>
         </is>
       </c>
     </row>
@@ -6943,6 +6873,11 @@
           <t>****** Prepare liquid cultivation medium for transformation</t>
         </is>
       </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>https://hub.ibisba.eu/sops/56</t>
+        </is>
+      </c>
       <c r="H136" t="inlineStr">
         <is>
           <t>NULL</t>
@@ -6958,7 +6893,7 @@
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>2019-06-14 13:08:05</t>
+          <t>2019-10-11 11:28:03</t>
         </is>
       </c>
     </row>
@@ -6977,6 +6912,11 @@
           <t>****** Prepare solid cultivation medium for transformation</t>
         </is>
       </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>https://hub.ibisba.eu/sops/55</t>
+        </is>
+      </c>
       <c r="H137" t="inlineStr">
         <is>
           <t>NULL</t>
@@ -6992,7 +6932,7 @@
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>2019-06-14 13:09:22</t>
+          <t>2019-10-11 11:32:47</t>
         </is>
       </c>
     </row>
@@ -7079,6 +7019,11 @@
           <t>****** Make glycerol stock</t>
         </is>
       </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>https://hub.ibisba.eu/sops/54</t>
+        </is>
+      </c>
       <c r="H140" t="inlineStr">
         <is>
           <t>NULL</t>
@@ -7094,7 +7039,7 @@
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>2019-06-14 13:08:05</t>
+          <t>2019-10-11 11:35:20</t>
         </is>
       </c>
     </row>
@@ -7260,22 +7205,12 @@
           <t>***** In vitro assembly of the DNA construct</t>
         </is>
       </c>
-      <c r="F144" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>https://drive.google.com/open?id=1zPZF2czFpIIf8-Z2ntBj1nXWQtfg6FgY</t>
+          <t>https://hub.ibisba.eu/sops/52</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="I144" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -7290,7 +7225,7 @@
       </c>
       <c r="M144" t="inlineStr">
         <is>
-          <t>2019-03-28 15:17:24</t>
+          <t>2019-10-11 11:41:13</t>
         </is>
       </c>
     </row>
@@ -7353,17 +7288,12 @@
           <t>****** Prepare cultivation media for transformation</t>
         </is>
       </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>NULL</t>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>https://hub.ibisba.eu/sops/56</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="I146" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -7378,7 +7308,7 @@
       </c>
       <c r="M146" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>2019-10-11 11:30:51</t>
         </is>
       </c>
     </row>
@@ -7834,25 +7764,15 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>****** Make glycerol stock #SopNeeded</t>
-        </is>
-      </c>
-      <c r="F157" t="inlineStr">
-        <is>
-          <t>NULL</t>
+          <t>****** Make glycerol stock</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>https://drive.google.com/open?id=1y80SYGUnF9VDrgF09_izEyBXnyFljOuAI7SUn1FV1Is</t>
+          <t>https://hub.ibisba.eu/sops/54, https://hub.ibisba.eu/sops/53</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="I157" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -7867,7 +7787,7 @@
       </c>
       <c r="M157" t="inlineStr">
         <is>
-          <t>2019-03-28 11:09:00</t>
+          <t>2019-10-11 13:05:31</t>
         </is>
       </c>
     </row>
@@ -7883,20 +7803,10 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>****** Add label/barcode #SopNeeded</t>
-        </is>
-      </c>
-      <c r="F158" t="inlineStr">
-        <is>
-          <t>NULL</t>
+          <t>****** Add label/barcode</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="I158" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -7911,7 +7821,7 @@
       </c>
       <c r="M158" t="inlineStr">
         <is>
-          <t>2019-03-25 08:49:12</t>
+          <t>2019-10-11 13:05:45</t>
         </is>
       </c>
     </row>
@@ -7974,17 +7884,12 @@
           <t>**** In vitro assembly of the integration/expression vector</t>
         </is>
       </c>
-      <c r="F160" t="inlineStr">
-        <is>
-          <t>NULL</t>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>https://hub.ibisba.eu/sops/57</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="I160" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -7999,7 +7904,7 @@
       </c>
       <c r="M160" t="inlineStr">
         <is>
-          <t>2019-04-03 14:15:16</t>
+          <t>2019-10-11 11:41:31</t>
         </is>
       </c>
     </row>
@@ -8551,17 +8456,12 @@
           <t>****** Make glycerol stock</t>
         </is>
       </c>
-      <c r="F173" t="inlineStr">
-        <is>
-          <t>NULL</t>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>https://hub.ibisba.eu/sops/54, https://hub.ibisba.eu/sops/53</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="I173" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -8576,7 +8476,7 @@
       </c>
       <c r="M173" t="inlineStr">
         <is>
-          <t>2019-04-10 07:59:18</t>
+          <t>2019-10-11 11:37:35</t>
         </is>
       </c>
     </row>
@@ -8870,14 +8770,9 @@
           <t>***** Prepare genetic material for transformation</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>https://drive.google.com/open?id=1SwFf5E5D0nY5IGD8epUa7Vkc-9x1z3Oe</t>
+          <t>https://hub.ibisba.eu/sops/51</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
@@ -8885,11 +8780,6 @@
           <t>NULL</t>
         </is>
       </c>
-      <c r="I179" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="J179" t="inlineStr">
         <is>
           <t>#SopNeeded for use of restriction enzymes</t>
@@ -8905,7 +8795,7 @@
       </c>
       <c r="M179" t="inlineStr">
         <is>
-          <t>2019-03-28 14:24:26</t>
+          <t>2019-10-11 11:38:22</t>
         </is>
       </c>
     </row>
@@ -9780,22 +9670,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>**** Recombinant clone screening and selection (depends on transformation implementation) #SopNeeded</t>
-        </is>
-      </c>
-      <c r="E196" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="F196" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="G196" t="inlineStr">
-        <is>
-          <t>NULL</t>
+          <t>**** Recombinant clone screening and selection (depends on transformation implementation)</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -9803,11 +9678,6 @@
           <t>NULL</t>
         </is>
       </c>
-      <c r="I196" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="K196" t="inlineStr">
         <is>
           <t>NULL</t>
@@ -9818,7 +9688,7 @@
       </c>
       <c r="M196" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>2019-10-11 13:07:27</t>
         </is>
       </c>
     </row>
@@ -9940,14 +9810,9 @@
           <t>***** Make glycerol stock #SopNeeded</t>
         </is>
       </c>
-      <c r="F199" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>https://drive.google.com/open?id=1pK3pXq2jPZ2fWxcDbK1wWvWpG6NWo7La</t>
+          <t>https://hub.ibisba.eu/sops/54, https://hub.ibisba.eu/sops/53</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -9955,11 +9820,6 @@
           <t>NULL</t>
         </is>
       </c>
-      <c r="I199" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
       <c r="K199" t="inlineStr">
         <is>
           <t>NULL</t>
@@ -9970,7 +9830,7 @@
       </c>
       <c r="M199" t="inlineStr">
         <is>
-          <t>2019-03-28 11:07:14</t>
+          <t>2019-10-11 11:39:11</t>
         </is>
       </c>
     </row>

</xml_diff>